<commit_message>
Mudanças para a importação e envio de eventos R4010
</commit_message>
<xml_diff>
--- a/cypress/fixtures/4020OpenTeste.xlsx
+++ b/cypress/fixtures/4020OpenTeste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe Mitre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe Mitre\Documents\CypressOpen2.3.2\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C047CAC-4AE4-4072-95FE-27FD69B870D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AF30A3-D8D4-4927-8592-99D3997C4AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,9 +991,9 @@
   </sheetPr>
   <dimension ref="A1:AD134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1137,10 +1137,10 @@
         <v>26</v>
       </c>
       <c r="D3" s="15">
-        <v>45861</v>
+        <v>45892</v>
       </c>
       <c r="E3" s="15">
-        <v>45868</v>
+        <v>45899</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>27</v>

</xml_diff>